<commit_message>
this added report last 11-11-24
</commit_message>
<xml_diff>
--- a/DD-Profit_ROI/Mangrove Oct-24 Profit and Loss.xlsx
+++ b/DD-Profit_ROI/Mangrove Oct-24 Profit and Loss.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mangrove\DD-Profit_ROI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaki\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFABEF9-C406-4750-ABBD-4ADDE4444EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DA889F-51E6-49D7-B266-E465F343E145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Variable Salary</t>
   </si>
   <si>
-    <t>Eid Bonus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mobile Bill If any </t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Total Other Expenses</t>
+  </si>
+  <si>
+    <t>Puja Bonus</t>
   </si>
 </sst>
 </file>
@@ -689,24 +689,6 @@
   </cellStyleXfs>
   <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -721,24 +703,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -747,12 +711,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,15 +749,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -839,12 +788,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,81 +795,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -951,6 +819,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1232,10 +1232,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,606 +1253,609 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="73"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="2">
         <v>45589</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="10"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="30">
-        <v>4233405</v>
-      </c>
-      <c r="C11" s="31">
+      <c r="B11" s="16">
+        <v>3005747</v>
+      </c>
+      <c r="C11" s="17">
         <f>B11*0.01</f>
-        <v>42334.05</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
+        <v>30057.47</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="30">
-        <v>1331008</v>
-      </c>
-      <c r="C12" s="31">
+      <c r="B12" s="16">
+        <v>1689212</v>
+      </c>
+      <c r="C12" s="17">
         <f>B12*0.01</f>
-        <v>13310.08</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="10"/>
+        <v>16892.12</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30">
-        <v>4752</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="10"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30">
-        <v>24750</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16">
+        <f>11250+21500</f>
+        <v>32750</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="30">
-        <v>400</v>
-      </c>
-      <c r="C16" s="30">
+      <c r="B16" s="16">
+        <v>100</v>
+      </c>
+      <c r="C16" s="16">
         <f>B16*9</f>
-        <v>3600</v>
-      </c>
-      <c r="G16" s="33"/>
+        <v>900</v>
+      </c>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="21">
         <v>0</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="21">
         <f>SUM(C11:C16)</f>
-        <v>88746.13</v>
-      </c>
-      <c r="G17" s="33"/>
+        <v>85599.59</v>
+      </c>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="G18" s="33"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="G19" s="33"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="G20" s="33"/>
+      <c r="A20" s="24"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="41"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="41"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="41"/>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A23" s="82"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="84"/>
+    </row>
+    <row r="24" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="F24" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="G24" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="44" t="s">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="30">
         <f t="shared" ref="G25:G35" si="0">SUM(B25:F25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="46">
+      <c r="A26" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="29">
         <v>10000</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47">
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29">
+        <v>10000</v>
+      </c>
+      <c r="D27" s="29">
+        <v>9000</v>
+      </c>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30">
+        <f t="shared" si="0"/>
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46">
-        <v>10000</v>
-      </c>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47">
-        <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="46">
+      <c r="B28" s="29">
         <v>13000</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47">
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30">
         <f t="shared" si="0"/>
         <v>13000</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47">
+      <c r="A29" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="46">
+      <c r="A30" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="29">
         <v>7000</v>
       </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47">
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47">
+      <c r="A31" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47">
+      <c r="A32" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="47">
+      <c r="A33" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="47">
+      <c r="A34" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="49">
+      <c r="A35" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="32">
         <v>1000</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50">
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36">
+        <f>SUM(G25:G35)</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
+    </row>
+    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="53">
-        <f>SUM(G25:G35)</f>
-        <v>41000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="56"/>
-    </row>
-    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
+      <c r="B39" s="86"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="39"/>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="58"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="56"/>
-    </row>
-    <row r="40" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="59" t="s">
+      <c r="B40" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="D40" s="37"/>
+      <c r="G40" s="39"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="54"/>
-      <c r="G40" s="56"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
+      <c r="B41" s="42">
+        <v>14820</v>
+      </c>
+      <c r="C41" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="61">
-        <v>14100</v>
-      </c>
-      <c r="C41" s="62" t="s">
+      <c r="D41" s="88"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="93">
+        <f>G36+B51</f>
+        <v>85572</v>
+      </c>
+      <c r="G41" s="94"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="63"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="65">
-        <f>G36+B51</f>
-        <v>85921</v>
-      </c>
-      <c r="G41" s="66"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="45" t="s">
+      <c r="B42" s="42">
+        <v>8000</v>
+      </c>
+      <c r="C42" s="90"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="95"/>
+      <c r="G42" s="96"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="61">
-        <v>8000</v>
-      </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="71"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="45" t="s">
+      <c r="B43" s="42"/>
+      <c r="C43" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="61"/>
-      <c r="C43" s="72" t="s">
+      <c r="D43" s="54"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="62">
+        <f>C17-F41</f>
+        <v>27.589999999996508</v>
+      </c>
+      <c r="G43" s="63"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="75">
-        <f>C17-F41</f>
-        <v>2825.1300000000047</v>
-      </c>
-      <c r="G43" s="76"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="45" t="s">
+      <c r="B44" s="42">
+        <v>700</v>
+      </c>
+      <c r="C44" s="56"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="61">
-        <v>700</v>
-      </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="81"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+      <c r="B45" s="42">
+        <f>7370-5500</f>
+        <v>1870</v>
+      </c>
+      <c r="C45" s="59"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="67"/>
+    </row>
+    <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A46" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="61">
-        <v>5670</v>
-      </c>
-      <c r="C45" s="82"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="86"/>
-    </row>
-    <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A46" s="87" t="s">
+      <c r="B46" s="44">
+        <v>5060</v>
+      </c>
+      <c r="F46" s="45"/>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="88">
-        <v>5560</v>
-      </c>
-      <c r="F46" s="89"/>
-      <c r="G46" s="33"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="90" t="s">
+      <c r="B47" s="47">
+        <v>1940</v>
+      </c>
+      <c r="G47" s="19"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="91">
-        <v>800</v>
-      </c>
-      <c r="G47" s="33"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="90" t="s">
+      <c r="B48" s="47">
+        <v>110</v>
+      </c>
+      <c r="E48" s="38"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="91">
-        <v>110</v>
-      </c>
-      <c r="E48" s="55"/>
-      <c r="G48" s="33"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="87" t="s">
+      <c r="B49" s="44"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="88">
-        <v>9200</v>
-      </c>
-      <c r="G49" s="33"/>
-    </row>
-    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="92" t="s">
+      <c r="B50" s="47">
+        <f>4472-1400</f>
+        <v>3072</v>
+      </c>
+      <c r="G50" s="19"/>
+    </row>
+    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="91">
-        <v>781</v>
-      </c>
-      <c r="G50" s="33"/>
-    </row>
-    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="93">
+      <c r="B51" s="49">
         <f>SUM(B41:B50)</f>
-        <v>44921</v>
-      </c>
-      <c r="G51" s="33"/>
+        <v>35572</v>
+      </c>
+      <c r="G51" s="19"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="94"/>
-      <c r="B52" s="95"/>
-      <c r="C52" s="95"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="95"/>
-      <c r="F52" s="95"/>
-      <c r="G52" s="96"/>
+      <c r="A52" s="50"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1864,5 +1870,6 @@
     <mergeCell ref="F41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>